<commit_message>
feat: correções nas tabelas fato e dimensão a serem utilizados no desafio técnico
</commit_message>
<xml_diff>
--- a/dim_inspetores.xlsx
+++ b/dim_inspetores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sipel\Documents\preparacao-desafios-sipel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39CE5C43-447C-4937-A27E-4072DDDD085C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FC01F78-C221-4DAB-BBB4-5A8ABB6EDCE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="16440" xr2:uid="{7435B823-D058-48F3-8F94-EDAB4B4FAC16}"/>
+    <workbookView xWindow="-22046" yWindow="-2254" windowWidth="22149" windowHeight="13920" xr2:uid="{7435B823-D058-48F3-8F94-EDAB4B4FAC16}"/>
   </bookViews>
   <sheets>
     <sheet name="dim_insp" sheetId="1" r:id="rId1"/>
@@ -42,132 +42,6 @@
     <t>Setor</t>
   </si>
   <si>
-    <t xml:space="preserve">VALQUÍRIA ALVES TAVARES </t>
-  </si>
-  <si>
-    <t xml:space="preserve">JOSE CARDOSO DA SILVA </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ALICE DOS SANTOS CRUZ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ALQUIDEAS GONCALVES DA SILVA FILHO </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ELVES PEDRO DA SILVA FERREIRA </t>
-  </si>
-  <si>
-    <t xml:space="preserve">LUCAS SANTANA ALVES </t>
-  </si>
-  <si>
-    <t xml:space="preserve">JOSSIANE SILVA RIBEIRO </t>
-  </si>
-  <si>
-    <t xml:space="preserve">JAQUELINE SILVA DE OLIVEIRA </t>
-  </si>
-  <si>
-    <t xml:space="preserve">FRANK WILLIAN DOS SANTOS COSTA </t>
-  </si>
-  <si>
-    <t xml:space="preserve">LUIZ PAULO BATISTA DOS SANTOS </t>
-  </si>
-  <si>
-    <t xml:space="preserve">DIOGO WESLEY OLIVEIRA NASCIMENTO </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ACACIO DA SILVA ANDRADE </t>
-  </si>
-  <si>
-    <t xml:space="preserve">TULIO ALEXANDRE SILVEIRA DA SILVA </t>
-  </si>
-  <si>
-    <t xml:space="preserve">PAULO JUNIOR DOS SANTOS DIAS </t>
-  </si>
-  <si>
-    <t xml:space="preserve">EDIE JONNES SILVA OLIVEIRA </t>
-  </si>
-  <si>
-    <t xml:space="preserve">JOAO PAULO MIRANDA DE PAULA </t>
-  </si>
-  <si>
-    <t xml:space="preserve">MARCOS FELIX DA SILVA FIGUEIREDO </t>
-  </si>
-  <si>
-    <t xml:space="preserve">JOSE RENER NUNES BEZERRA </t>
-  </si>
-  <si>
-    <t xml:space="preserve">AISLAN OLIVEIRA DOS SANTOS </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANDRE MARQUES DA SILVA </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANDERSON MOREIRA DA SILVA JUNIOR </t>
-  </si>
-  <si>
-    <t xml:space="preserve">GABRIEL NASCIMENTO SANTOS </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SANDRO SANTIAGO OLIVEIRA  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANDERSON SANTOS DE OLIVEIRA </t>
-  </si>
-  <si>
-    <t xml:space="preserve">MARA MILENE DE BRITO NEVES </t>
-  </si>
-  <si>
-    <t xml:space="preserve">RAFAEL BERNARDO MAGALHAES </t>
-  </si>
-  <si>
-    <t xml:space="preserve">IANI CHAGAS MIRANDA </t>
-  </si>
-  <si>
-    <t xml:space="preserve">WESLEY DE ARAUJO ROCHA </t>
-  </si>
-  <si>
-    <t xml:space="preserve">GUSTAVO PEREIRA DOS SANTOS </t>
-  </si>
-  <si>
-    <t xml:space="preserve">EDCLECIO OLIVEIRA DE LIMA </t>
-  </si>
-  <si>
-    <t xml:space="preserve">EDLECIO ELIAS MAGALHAES </t>
-  </si>
-  <si>
-    <t xml:space="preserve">JOSE WELLINGTON DE JESUS SANTOS </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ALAN SANTOS MOURA </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANTONIO CARLOS JESUS DE MENEZES </t>
-  </si>
-  <si>
-    <t xml:space="preserve">FRANKLYN HENRIQUE DOS SANTOS COSTA </t>
-  </si>
-  <si>
-    <t xml:space="preserve">GABRIEL MIRANDA DA SILVA BERTORA </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANTONIO FELIX DOS SANTOS TAVARES </t>
-  </si>
-  <si>
-    <t xml:space="preserve">JESSICA DO NASCIMENTO SOUZA </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ELIEZER DOS SANTOS </t>
-  </si>
-  <si>
-    <t xml:space="preserve">MICHEL DE SOUZA RAMOS </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CLEITISVAL XAVIER COELHO </t>
-  </si>
-  <si>
-    <t xml:space="preserve">MAGALI CORREA DA SILVA </t>
-  </si>
-  <si>
     <t>Jacobina</t>
   </si>
   <si>
@@ -187,6 +61,132 @@
   </si>
   <si>
     <t>Comercial</t>
+  </si>
+  <si>
+    <t>ACACIO DA SILVA ANDRADE</t>
+  </si>
+  <si>
+    <t>AISLAN OLIVEIRA DOS SANTOS</t>
+  </si>
+  <si>
+    <t>ALAN SANTOS MOURA</t>
+  </si>
+  <si>
+    <t>ALICE DOS SANTOS CRUZ</t>
+  </si>
+  <si>
+    <t>ALQUIDEAS GONCALVES DA SILVA FILHO</t>
+  </si>
+  <si>
+    <t>ANDERSON MOREIRA DA SILVA JUNIOR</t>
+  </si>
+  <si>
+    <t>ANDERSON SANTOS DE OLIVEIRA</t>
+  </si>
+  <si>
+    <t>ANDRE MARQUES DA SILVA</t>
+  </si>
+  <si>
+    <t>ANTONIO CARLOS JESUS DE MENEZES</t>
+  </si>
+  <si>
+    <t>ANTONIO FELIX DOS SANTOS TAVARES</t>
+  </si>
+  <si>
+    <t>CLEITISVAL XAVIER COELHO</t>
+  </si>
+  <si>
+    <t>DIOGO WESLEY OLIVEIRA NASCIMENTO</t>
+  </si>
+  <si>
+    <t>EDCLECIO OLIVEIRA DE LIMA</t>
+  </si>
+  <si>
+    <t>EDIE JONNES SILVA OLIVEIRA</t>
+  </si>
+  <si>
+    <t>EDLECIO ELIAS MAGALHAES</t>
+  </si>
+  <si>
+    <t>ELIEZER DOS SANTOS</t>
+  </si>
+  <si>
+    <t>ELVES PEDRO DA SILVA FERREIRA</t>
+  </si>
+  <si>
+    <t>FRANK WILLIAN DOS SANTOS COSTA</t>
+  </si>
+  <si>
+    <t>FRANKLYN HENRIQUE DOS SANTOS COSTA</t>
+  </si>
+  <si>
+    <t>GABRIEL MIRANDA DA SILVA BERTORA</t>
+  </si>
+  <si>
+    <t>GABRIEL NASCIMENTO SANTOS</t>
+  </si>
+  <si>
+    <t>GUSTAVO PEREIRA DOS SANTOS</t>
+  </si>
+  <si>
+    <t>IANI CHAGAS MIRANDA</t>
+  </si>
+  <si>
+    <t>JAQUELINE SILVA DE OLIVEIRA</t>
+  </si>
+  <si>
+    <t>JESSICA DO NASCIMENTO SOUZA</t>
+  </si>
+  <si>
+    <t>JOAO PAULO MIRANDA DE PAULA</t>
+  </si>
+  <si>
+    <t>JOSE CARDOSO DA SILVA</t>
+  </si>
+  <si>
+    <t>JOSE RENER NUNES BEZERRA</t>
+  </si>
+  <si>
+    <t>JOSE WELLINGTON DE JESUS SANTOS</t>
+  </si>
+  <si>
+    <t>JOSSIANE SILVA RIBEIRO</t>
+  </si>
+  <si>
+    <t>LUCAS SANTANA ALVES</t>
+  </si>
+  <si>
+    <t>LUIZ PAULO BATISTA DOS SANTOS</t>
+  </si>
+  <si>
+    <t>MAGALI CORREA DA SILVA</t>
+  </si>
+  <si>
+    <t>MARA MILENE DE BRITO NEVES</t>
+  </si>
+  <si>
+    <t>MARCOS FELIX DA SILVA FIGUEIREDO</t>
+  </si>
+  <si>
+    <t>MICHEL DE SOUZA RAMOS</t>
+  </si>
+  <si>
+    <t>PAULO JUNIOR DOS SANTOS DIAS</t>
+  </si>
+  <si>
+    <t>RAFAEL BERNARDO MAGALHAES</t>
+  </si>
+  <si>
+    <t>SANDRO SANTIAGO OLIVEIRA</t>
+  </si>
+  <si>
+    <t>TULIO ALEXANDRE SILVEIRA DA SILVA</t>
+  </si>
+  <si>
+    <t>VALQUÍRIA ALVES TAVARES</t>
+  </si>
+  <si>
+    <t>WESLEY DE ARAUJO ROCHA</t>
   </si>
 </sst>
 </file>
@@ -546,7 +546,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95456A22-56F0-4AFE-98F0-C4D8DE1BA083}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -575,13 +577,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>49</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -589,13 +591,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>49</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -603,13 +605,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>50</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -617,13 +619,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
+        <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -631,13 +633,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
         <v>7</v>
-      </c>
-      <c r="C6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D6" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -645,13 +647,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>52</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -659,13 +661,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>47</v>
+        <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>50</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -673,13 +675,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>47</v>
+        <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -687,13 +689,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>49</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -701,13 +703,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>49</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -715,13 +717,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>47</v>
+        <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>50</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -729,13 +731,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>47</v>
+        <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>49</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -743,13 +745,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>50</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -757,13 +759,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C15" t="s">
-        <v>47</v>
+        <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>50</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -771,13 +773,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C16" t="s">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="D16" t="s">
-        <v>50</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -785,13 +787,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="C17" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>50</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -799,13 +801,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="C18" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>52</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -813,13 +815,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="C19" t="s">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="D19" t="s">
-        <v>49</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -827,13 +829,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C20" t="s">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="D20" t="s">
-        <v>52</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -841,13 +843,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="C21" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>50</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -855,13 +857,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C22" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>52</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -872,10 +874,10 @@
         <v>32</v>
       </c>
       <c r="C23" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>52</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -883,13 +885,13 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C24" t="s">
-        <v>47</v>
+        <v>5</v>
       </c>
       <c r="D24" t="s">
-        <v>52</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -897,13 +899,13 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="C25" t="s">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="D25" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -911,13 +913,13 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C26" t="s">
-        <v>47</v>
+        <v>5</v>
       </c>
       <c r="D26" t="s">
-        <v>52</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -925,13 +927,13 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="C27" t="s">
-        <v>47</v>
+        <v>5</v>
       </c>
       <c r="D27" t="s">
-        <v>52</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -939,13 +941,13 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="C28" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -953,13 +955,13 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="C29" t="s">
-        <v>47</v>
+        <v>5</v>
       </c>
       <c r="D29" t="s">
-        <v>49</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -967,13 +969,13 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C30" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="D30" t="s">
-        <v>49</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -981,13 +983,13 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="C31" t="s">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="D31" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -995,13 +997,13 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="C32" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="D32" t="s">
-        <v>49</v>
+        <v>7</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1009,13 +1011,13 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="C33" t="s">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="D33" t="s">
-        <v>52</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1023,13 +1025,13 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C34" t="s">
-        <v>47</v>
+        <v>5</v>
       </c>
       <c r="D34" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1037,13 +1039,13 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="C35" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="D35" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1051,13 +1053,13 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="C36" t="s">
-        <v>47</v>
+        <v>5</v>
       </c>
       <c r="D36" t="s">
-        <v>52</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1065,13 +1067,13 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C37" t="s">
-        <v>47</v>
+        <v>5</v>
       </c>
       <c r="D37" t="s">
-        <v>50</v>
+        <v>8</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1079,13 +1081,13 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="C38" t="s">
-        <v>47</v>
+        <v>5</v>
       </c>
       <c r="D38" t="s">
-        <v>50</v>
+        <v>8</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1093,13 +1095,13 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="C39" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="D39" t="s">
-        <v>50</v>
+        <v>8</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1107,13 +1109,13 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="C40" t="s">
-        <v>47</v>
+        <v>5</v>
       </c>
       <c r="D40" t="s">
-        <v>50</v>
+        <v>8</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1121,13 +1123,13 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="C41" t="s">
-        <v>47</v>
+        <v>5</v>
       </c>
       <c r="D41" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1135,13 +1137,13 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>4</v>
+        <v>51</v>
       </c>
       <c r="C42" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="D42" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1149,13 +1151,13 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="C43" t="s">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="D43" t="s">
-        <v>50</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>